<commit_message>
Selection Box fonctionnelle et testée
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -27,7 +27,10 @@
     <t>Entrée</t>
   </si>
   <si>
-    <t xml:space="preserve">Le développement de l'interface graphique prend plus de temps que prévu, cependant la partie "Chargeur de fichiers" va finalement être abandonnée, car Tkinter rend le processur plus facile que prévu. </t>
+    <t xml:space="preserve">Le développement de l'interface graphique prend plus de temps que prévu, cependant la partie "Chargeur de fichiers" va finalement être abandonnée, car le processus est moins complexe que prévu. </t>
+  </si>
+  <si>
+    <t>Après entretien avec M. Ithurbide, il a été décidé que la méthode de prendre un screenshot n'était effectivement pas optimisée, ou portable (celle-ci utilisait notamment un offset de coordonées hardodé, prévu pour ignorer spécifiquement les bordures de fenêtres windows 7). À la place, une conversion de l'image en matrice numpy sera utilisée</t>
   </si>
 </sst>
 </file>
@@ -345,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,6 +375,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23.05</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Gestion des images en POO
Désormais, quand on charge une image, un objet correspondant est créé, contenant ses infos (origine, largeur, hauteur, ...), et des methodes relevantes (sauvegarder, afficher sur le canvas, ...)
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Après entretien avec M. Ithurbide, il a été décidé que la méthode de prendre un screenshot n'était effectivement pas optimisée, ou portable (celle-ci utilisait notamment un offset de coordonées hardodé, prévu pour ignorer spécifiquement les bordures de fenêtres windows 7). À la place, une conversion de l'image en matrice numpy sera utilisée</t>
+  </si>
+  <si>
+    <t>J'ai passé la matinée sur un problème passablement frustrant. En essayant de modifier le chargeur d'image pour le faire créer des objets, j'ai oublié de convertir Image.fromarray(image) en ImageTk.PhotoImage. Problème résolu, mais du temps a été perdu inutilement sur un problème facile. Cependant, avec la nouvelle architecture orientée objet, il me sera plus facile de récupérer une partie de l'image.</t>
   </si>
 </sst>
 </file>
@@ -348,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,6 +386,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>24.05</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Récupération d'une partie de la matrice ok
Enregistrement sans sélection ok. bonnes coordonnées passées à l'objet NumpyImage
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$28</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -34,15 +37,42 @@
   </si>
   <si>
     <t>J'ai passé la matinée sur un problème passablement frustrant. En essayant de modifier le chargeur d'image pour le faire créer des objets, j'ai oublié de convertir Image.fromarray(image) en ImageTk.PhotoImage. Problème résolu, mais du temps a été perdu inutilement sur un problème facile. Cependant, avec la nouvelle architecture orientée objet, il me sera plus facile de récupérer une partie de l'image.</t>
+  </si>
+  <si>
+    <t>Note à moi-même: Il aurait été bien plus simple d'empêcher le retournement de la selection_box,  par exemple en swappant le côté sélectionné quand la souris passe au dessus, car il est complexe de transformer des coordonnées négatives, et une boite de sélection basée sur des valeurs width et height.</t>
+  </si>
+  <si>
+    <t>Journal de bord</t>
+  </si>
+  <si>
+    <t>Jeremy Comelli</t>
+  </si>
+  <si>
+    <t>Après discussions avec M. Ithurbide, je me suis rendu compte que j'ai failli partir sur une feature qui ne se trouvait pas dans le cahier des charges (le collage d'images, qui se fera avec programme tiers, comme photoshop). Il a aussi été décidé de développer le recadrage, et d'implémenter le processing d'images à travers des matrices numpy.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -57,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -65,12 +95,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,50 +509,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="189.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="156.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>43269</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>17.05</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="7" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>23.05</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>24.05</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>24.05</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>24.05</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="2.0866141732283467" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>